<commit_message>
running from a new suite
</commit_message>
<xml_diff>
--- a/src/test/resources/testCases.xlsx
+++ b/src/test/resources/testCases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
   <si>
     <t>Initial Testcase Excel</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>author</t>
+  </si>
+  <si>
+    <t>bug_2020_user1</t>
   </si>
   <si>
     <t>Pass</t>
@@ -2267,7 +2270,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:I15"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -2278,8 +2281,8 @@
     <col min="1" max="1" width="22.3047" style="39" customWidth="1"/>
     <col min="2" max="6" width="16.3516" style="39" customWidth="1"/>
     <col min="7" max="7" width="19.625" style="39" customWidth="1"/>
-    <col min="8" max="9" width="16.3516" style="39" customWidth="1"/>
-    <col min="10" max="16384" width="16.3516" style="39" customWidth="1"/>
+    <col min="8" max="10" width="16.3516" style="39" customWidth="1"/>
+    <col min="11" max="16384" width="16.3516" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -2294,6 +2297,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" ht="20.45" customHeight="1">
       <c r="A2" t="s" s="3">
@@ -2320,8 +2324,11 @@
       <c r="H2" t="s" s="19">
         <v>28</v>
       </c>
-      <c r="I2" t="s" s="40">
+      <c r="I2" t="s" s="19">
         <v>29</v>
+      </c>
+      <c r="J2" t="s" s="40">
+        <v>30</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
@@ -2344,14 +2351,15 @@
         <v>7</v>
       </c>
       <c r="G3" t="s" s="24">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="41">
         <v>0</v>
       </c>
       <c r="I3" t="s" s="24">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J3" s="27"/>
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="29">
@@ -2373,14 +2381,15 @@
         <v>4</v>
       </c>
       <c r="G4" t="s" s="43">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H4" s="44">
         <v>3</v>
       </c>
       <c r="I4" t="s" s="30">
-        <v>33</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="33">
@@ -2402,14 +2411,15 @@
         <v>4</v>
       </c>
       <c r="G5" t="s" s="43">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="45">
         <v>5</v>
       </c>
       <c r="I5" t="s" s="34">
-        <v>33</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J5" s="35"/>
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" t="s" s="29">
@@ -2431,13 +2441,16 @@
         <v>7</v>
       </c>
       <c r="G6" t="s" s="30">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H6" s="44">
         <v>0</v>
       </c>
       <c r="I6" t="s" s="30">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="J6" t="s" s="30">
+        <v>4</v>
       </c>
     </row>
     <row r="7" ht="20.2" customHeight="1">
@@ -2460,13 +2473,16 @@
         <v>7</v>
       </c>
       <c r="G7" t="s" s="34">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" s="45">
         <v>0</v>
       </c>
       <c r="I7" t="s" s="34">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="J7" t="s" s="34">
+        <v>4</v>
       </c>
     </row>
     <row r="8" ht="20.2" customHeight="1">
@@ -2489,13 +2505,16 @@
         <v>7</v>
       </c>
       <c r="G8" t="s" s="43">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H8" s="44">
         <v>1</v>
       </c>
       <c r="I8" t="s" s="30">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="J8" t="s" s="30">
+        <v>4</v>
       </c>
     </row>
     <row r="9" ht="20.2" customHeight="1">
@@ -2518,14 +2537,15 @@
         <v>7</v>
       </c>
       <c r="G9" t="s" s="34">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H9" s="45">
         <v>0</v>
       </c>
       <c r="I9" t="s" s="34">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
       <c r="A10" t="s" s="29">
@@ -2547,14 +2567,15 @@
         <v>7</v>
       </c>
       <c r="G10" t="s" s="30">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H10" s="44">
         <v>0</v>
       </c>
       <c r="I10" t="s" s="30">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J10" s="31"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
       <c r="A11" t="s" s="33">
@@ -2576,14 +2597,15 @@
         <v>7</v>
       </c>
       <c r="G11" t="s" s="34">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H11" s="45">
         <v>0</v>
       </c>
       <c r="I11" t="s" s="34">
-        <v>31</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="J11" s="35"/>
     </row>
     <row r="12" ht="20.2" customHeight="1">
       <c r="A12" t="s" s="29">
@@ -2605,14 +2627,15 @@
         <v>7</v>
       </c>
       <c r="G12" t="s" s="30">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H12" s="44">
         <v>0</v>
       </c>
       <c r="I12" t="s" s="30">
-        <v>33</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J12" s="31"/>
     </row>
     <row r="13" ht="20.2" customHeight="1">
       <c r="A13" t="s" s="33">
@@ -2634,14 +2657,15 @@
         <v>7</v>
       </c>
       <c r="G13" t="s" s="34">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H13" s="45">
         <v>0</v>
       </c>
       <c r="I13" t="s" s="34">
-        <v>33</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="J13" s="35"/>
     </row>
     <row r="14" ht="20.2" customHeight="1">
       <c r="A14" s="32"/>
@@ -2653,6 +2677,7 @@
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
     </row>
     <row r="15" ht="20.2" customHeight="1">
       <c r="A15" s="36"/>
@@ -2664,10 +2689,11 @@
       <c r="G15" s="35"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>